<commit_message>
Initial version for goals
</commit_message>
<xml_diff>
--- a/doc/12.25.2013 Meeting/Result12.05.2013.xlsx
+++ b/doc/12.25.2013 Meeting/Result12.05.2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="33">
   <si>
     <t xml:space="preserve">Accuracy </t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>2waymodel_actngram_request_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binaryswitch_fullscore_topline </t>
+  </si>
+  <si>
+    <t xml:space="preserve">binaryswitch_fullscore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstcorrect </t>
   </si>
 </sst>
 </file>
@@ -179,9 +188,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -196,6 +202,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -512,16 +521,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -976,20 +985,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:AA24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="25" max="25" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1009,25 +1020,22 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s">
-        <v>17</v>
       </c>
       <c r="P1" t="s">
         <v>18</v>
@@ -1035,8 +1043,32 @@
       <c r="Q1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1055,35 +1087,56 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>8</v>
+      <c r="H2">
+        <v>0.54256899999999997</v>
       </c>
       <c r="I2">
+        <v>0.877525</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>0.6445419</v>
+      </c>
+      <c r="M2">
+        <v>0.68873660000000003</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2">
+        <v>0.68750549999999999</v>
+      </c>
+      <c r="Q2">
+        <v>0.62498900000000002</v>
+      </c>
+      <c r="S2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2">
+        <v>0.58763699999999996</v>
+      </c>
+      <c r="U2">
+        <v>0.82472599999999996</v>
+      </c>
+      <c r="W2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>0.54256899999999997</v>
-      </c>
-      <c r="K2">
-        <v>0.877525</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0.67338889999999996</v>
-      </c>
-      <c r="Q2">
-        <v>0.624776</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z2">
+        <v>0.58763699999999996</v>
+      </c>
+      <c r="AA2">
+        <v>0.82472599999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1102,35 +1155,56 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>8</v>
+      <c r="H3">
+        <v>0.55256470000000002</v>
       </c>
       <c r="I3">
+        <v>0.86342620000000003</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>0.65953530000000005</v>
+      </c>
+      <c r="M3">
+        <v>0.66027559999999996</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3">
+        <v>0.77045160000000001</v>
+      </c>
+      <c r="Q3">
+        <v>0.45909689999999997</v>
+      </c>
+      <c r="S3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3">
+        <v>0.57860590000000001</v>
+      </c>
+      <c r="U3">
+        <v>0.84278830000000005</v>
+      </c>
+      <c r="W3" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>0.55256470000000002</v>
-      </c>
-      <c r="K3">
-        <v>0.86342620000000003</v>
-      </c>
-      <c r="M3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>0.69302940000000002</v>
-      </c>
-      <c r="Q3">
-        <v>0.58965029999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z3">
+        <v>0.61516879999999996</v>
+      </c>
+      <c r="AA3">
+        <v>0.76966239999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1149,35 +1223,56 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
-        <v>8</v>
+      <c r="H4">
+        <v>0.55072339999999997</v>
       </c>
       <c r="I4">
+        <v>0.87090279999999998</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4">
+        <v>0.6631302</v>
+      </c>
+      <c r="M4">
+        <v>0.65535319999999997</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4">
+        <v>0.80008769999999996</v>
+      </c>
+      <c r="Q4">
+        <v>0.39982459999999997</v>
+      </c>
+      <c r="S4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4">
+        <v>0.54660240000000004</v>
+      </c>
+      <c r="U4">
+        <v>0.90679529999999997</v>
+      </c>
+      <c r="W4" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4">
         <v>2</v>
       </c>
-      <c r="J4">
-        <v>0.55072339999999997</v>
-      </c>
-      <c r="K4">
-        <v>0.87090279999999998</v>
-      </c>
-      <c r="M4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
-        <v>0.6960982</v>
-      </c>
-      <c r="Q4">
-        <v>0.58735269999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z4">
+        <v>0.61797460000000004</v>
+      </c>
+      <c r="AA4">
+        <v>0.76405089999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1196,35 +1291,56 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
-        <v>8</v>
+      <c r="H5">
+        <v>0.55177549999999997</v>
       </c>
       <c r="I5">
+        <v>0.87005200000000005</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>0.66497150000000005</v>
+      </c>
+      <c r="M5">
+        <v>0.65234979999999998</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5">
+        <v>0.81034629999999996</v>
+      </c>
+      <c r="Q5">
+        <v>0.37930730000000001</v>
+      </c>
+      <c r="S5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5">
+        <v>0.52301620000000004</v>
+      </c>
+      <c r="U5">
+        <v>0.95396760000000003</v>
+      </c>
+      <c r="W5" t="s">
+        <v>32</v>
+      </c>
+      <c r="X5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5">
         <v>3</v>
       </c>
-      <c r="J5">
-        <v>0.55177549999999997</v>
-      </c>
-      <c r="K5">
-        <v>0.87005200000000005</v>
-      </c>
-      <c r="M5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5">
-        <v>3</v>
-      </c>
-      <c r="P5">
-        <v>0.69715039999999995</v>
-      </c>
-      <c r="Q5">
-        <v>0.58590730000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z5">
+        <v>0.61885140000000005</v>
+      </c>
+      <c r="AA5">
+        <v>0.76229720000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1243,35 +1359,56 @@
       <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="H6" t="s">
-        <v>8</v>
+      <c r="H6">
+        <v>0.552477</v>
       </c>
       <c r="I6">
+        <v>0.8696374</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>0.66593599999999997</v>
+      </c>
+      <c r="M6">
+        <v>0.65124320000000002</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6">
+        <v>0.82007890000000006</v>
+      </c>
+      <c r="Q6">
+        <v>0.3598422</v>
+      </c>
+      <c r="S6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6">
+        <v>0.51591410000000004</v>
+      </c>
+      <c r="U6">
+        <v>0.96817189999999997</v>
+      </c>
+      <c r="W6" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y6">
         <v>4</v>
       </c>
-      <c r="J6">
-        <v>0.552477</v>
-      </c>
-      <c r="K6">
-        <v>0.8696374</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6">
-        <v>4</v>
-      </c>
-      <c r="P6">
-        <v>0.69802719999999996</v>
-      </c>
-      <c r="Q6">
-        <v>0.58455480000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z6">
+        <v>0.61920209999999998</v>
+      </c>
+      <c r="AA6">
+        <v>0.76159580000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1290,35 +1427,56 @@
       <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" t="s">
-        <v>8</v>
+      <c r="H7">
+        <v>0.55300309999999997</v>
       </c>
       <c r="I7">
+        <v>0.86857070000000003</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>0.66654979999999997</v>
+      </c>
+      <c r="M7">
+        <v>0.64998120000000004</v>
+      </c>
+      <c r="O7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7">
+        <v>0.82437530000000003</v>
+      </c>
+      <c r="Q7">
+        <v>0.35124949999999999</v>
+      </c>
+      <c r="S7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7">
+        <v>0.50977640000000002</v>
+      </c>
+      <c r="U7">
+        <v>0.98044719999999996</v>
+      </c>
+      <c r="W7" t="s">
+        <v>32</v>
+      </c>
+      <c r="X7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y7">
         <v>5</v>
       </c>
-      <c r="J7">
-        <v>0.55300309999999997</v>
-      </c>
-      <c r="K7">
-        <v>0.86857070000000003</v>
-      </c>
-      <c r="M7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7">
-        <v>5</v>
-      </c>
-      <c r="P7">
-        <v>0.69732570000000005</v>
-      </c>
-      <c r="Q7">
-        <v>0.58569930000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z7">
+        <v>0.61920209999999998</v>
+      </c>
+      <c r="AA7">
+        <v>0.76159580000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1337,35 +1495,56 @@
       <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" t="s">
-        <v>8</v>
+      <c r="H8">
+        <v>0.55352920000000005</v>
       </c>
       <c r="I8">
+        <v>0.86752039999999997</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>0.66760189999999997</v>
+      </c>
+      <c r="M8">
+        <v>0.64804119999999998</v>
+      </c>
+      <c r="O8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8">
+        <v>0.82612890000000005</v>
+      </c>
+      <c r="Q8">
+        <v>0.3477422</v>
+      </c>
+      <c r="S8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8">
+        <v>0.50618149999999995</v>
+      </c>
+      <c r="U8">
+        <v>0.98763699999999999</v>
+      </c>
+      <c r="W8" t="s">
+        <v>32</v>
+      </c>
+      <c r="X8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y8">
         <v>6</v>
       </c>
-      <c r="J8">
-        <v>0.55352920000000005</v>
-      </c>
-      <c r="K8">
-        <v>0.86752039999999997</v>
-      </c>
-      <c r="M8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O8">
-        <v>6</v>
-      </c>
-      <c r="P8">
-        <v>0.69890399999999997</v>
-      </c>
-      <c r="Q8">
-        <v>0.5825726</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z8">
+        <v>0.61972819999999995</v>
+      </c>
+      <c r="AA8">
+        <v>0.76054359999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1384,35 +1563,56 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" t="s">
-        <v>8</v>
+      <c r="H9">
+        <v>0.55352920000000005</v>
       </c>
       <c r="I9">
+        <v>0.86749189999999998</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9">
+        <v>0.66830339999999999</v>
+      </c>
+      <c r="M9">
+        <v>0.64670490000000003</v>
+      </c>
+      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9">
+        <v>0.8305129</v>
+      </c>
+      <c r="Q9">
+        <v>0.3389741</v>
+      </c>
+      <c r="S9" t="s">
+        <v>31</v>
+      </c>
+      <c r="T9">
+        <v>0.5051293</v>
+      </c>
+      <c r="U9">
+        <v>0.98974130000000005</v>
+      </c>
+      <c r="W9" t="s">
+        <v>32</v>
+      </c>
+      <c r="X9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y9">
         <v>7</v>
       </c>
-      <c r="J9">
-        <v>0.55352920000000005</v>
-      </c>
-      <c r="K9">
-        <v>0.86749189999999998</v>
-      </c>
-      <c r="M9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" t="s">
-        <v>8</v>
-      </c>
-      <c r="O9">
-        <v>7</v>
-      </c>
-      <c r="P9">
-        <v>0.69925470000000001</v>
-      </c>
-      <c r="Q9">
-        <v>0.58195149999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z9">
+        <v>0.61981589999999998</v>
+      </c>
+      <c r="AA9">
+        <v>0.7603683</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1431,35 +1631,56 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
-      <c r="H10" t="s">
-        <v>8</v>
+      <c r="H10">
+        <v>0.55352920000000005</v>
       </c>
       <c r="I10">
-        <v>8</v>
-      </c>
-      <c r="J10">
-        <v>0.55352920000000005</v>
-      </c>
-      <c r="K10">
         <v>0.86749310000000002</v>
       </c>
-      <c r="M10" t="s">
+      <c r="K10" t="s">
         <v>20</v>
       </c>
-      <c r="N10" t="s">
-        <v>8</v>
-      </c>
-      <c r="O10">
-        <v>8</v>
+      <c r="L10">
+        <v>0.66830339999999999</v>
+      </c>
+      <c r="M10">
+        <v>0.64670269999999996</v>
+      </c>
+      <c r="O10" t="s">
+        <v>30</v>
       </c>
       <c r="P10">
-        <v>0.69978079999999998</v>
+        <v>0.83138970000000001</v>
       </c>
       <c r="Q10">
-        <v>0.58087370000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.33722049999999998</v>
+      </c>
+      <c r="S10" t="s">
+        <v>31</v>
+      </c>
+      <c r="T10">
+        <v>0.50539239999999996</v>
+      </c>
+      <c r="U10">
+        <v>0.98921530000000002</v>
+      </c>
+      <c r="W10" t="s">
+        <v>32</v>
+      </c>
+      <c r="X10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10">
+        <v>8</v>
+      </c>
+      <c r="Z10">
+        <v>0.61981589999999998</v>
+      </c>
+      <c r="AA10">
+        <v>0.7603683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1478,35 +1699,56 @@
       <c r="G11" t="s">
         <v>14</v>
       </c>
-      <c r="H11" t="s">
-        <v>8</v>
+      <c r="H11">
+        <v>0.55352920000000005</v>
       </c>
       <c r="I11">
-        <v>9</v>
-      </c>
-      <c r="J11">
-        <v>0.55352920000000005</v>
-      </c>
-      <c r="K11">
         <v>0.86748950000000002</v>
       </c>
-      <c r="M11" t="s">
+      <c r="K11" t="s">
         <v>20</v>
       </c>
-      <c r="N11" t="s">
-        <v>8</v>
-      </c>
-      <c r="O11">
-        <v>9</v>
+      <c r="L11">
+        <v>0.66830339999999999</v>
+      </c>
+      <c r="M11">
+        <v>0.64669759999999998</v>
+      </c>
+      <c r="O11" t="s">
+        <v>30</v>
       </c>
       <c r="P11">
-        <v>0.69978079999999998</v>
+        <v>0.83138970000000001</v>
       </c>
       <c r="Q11">
-        <v>0.58088090000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.33722049999999998</v>
+      </c>
+      <c r="S11" t="s">
+        <v>31</v>
+      </c>
+      <c r="T11">
+        <v>0.50565539999999998</v>
+      </c>
+      <c r="U11">
+        <v>0.98868920000000005</v>
+      </c>
+      <c r="W11" t="s">
+        <v>32</v>
+      </c>
+      <c r="X11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y11">
+        <v>9</v>
+      </c>
+      <c r="Z11">
+        <v>0.61981589999999998</v>
+      </c>
+      <c r="AA11">
+        <v>0.7603683</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1525,82 +1767,56 @@
       <c r="G12" t="s">
         <v>14</v>
       </c>
-      <c r="H12" t="s">
-        <v>8</v>
+      <c r="H12">
+        <v>0.55352920000000005</v>
       </c>
       <c r="I12">
+        <v>0.86748950000000002</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <v>0.66830339999999999</v>
+      </c>
+      <c r="M12">
+        <v>0.64669759999999998</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12">
+        <v>0.83138970000000001</v>
+      </c>
+      <c r="Q12">
+        <v>0.33722049999999998</v>
+      </c>
+      <c r="S12" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12">
+        <v>0.50565539999999998</v>
+      </c>
+      <c r="U12">
+        <v>0.98868920000000005</v>
+      </c>
+      <c r="W12" t="s">
+        <v>32</v>
+      </c>
+      <c r="X12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y12">
         <v>10</v>
       </c>
-      <c r="J12">
-        <v>0.55352920000000005</v>
-      </c>
-      <c r="K12">
-        <v>0.86748950000000002</v>
-      </c>
-      <c r="M12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12" t="s">
-        <v>8</v>
-      </c>
-      <c r="O12">
-        <v>10</v>
-      </c>
-      <c r="P12">
-        <v>0.69978079999999998</v>
-      </c>
-      <c r="Q12">
-        <v>0.58088090000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0.54979140000000004</v>
-      </c>
-      <c r="E13">
-        <v>0.85786490000000004</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0.4619395</v>
-      </c>
-      <c r="K13">
-        <v>1.0193713</v>
-      </c>
-      <c r="M13" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0.58237749999999999</v>
-      </c>
-      <c r="Q13">
-        <v>0.78681319999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z12">
+        <v>0.61981589999999998</v>
+      </c>
+      <c r="AA12">
+        <v>0.7603683</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1608,46 +1824,67 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0.54144939999999997</v>
+        <v>0.54979140000000004</v>
       </c>
       <c r="E14">
-        <v>0.87640240000000003</v>
+        <v>0.85786490000000004</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
-      <c r="H14" t="s">
-        <v>9</v>
+      <c r="H14">
+        <v>0.4619395</v>
       </c>
       <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0.47888429999999998</v>
-      </c>
-      <c r="K14">
-        <v>0.99592639999999999</v>
-      </c>
-      <c r="M14" t="s">
+        <v>1.0193713</v>
+      </c>
+      <c r="K14" t="s">
         <v>20</v>
       </c>
-      <c r="N14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
+      <c r="L14">
+        <v>0.55344110000000002</v>
+      </c>
+      <c r="M14">
+        <v>0.85127730000000001</v>
+      </c>
+      <c r="O14" t="s">
+        <v>30</v>
       </c>
       <c r="P14">
-        <v>0.60192909999999999</v>
+        <v>0.60114699999999999</v>
       </c>
       <c r="Q14">
-        <v>0.75081940000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.79770589999999997</v>
+      </c>
+      <c r="S14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T14">
+        <v>0.51850890000000005</v>
+      </c>
+      <c r="U14">
+        <v>0.96298229999999996</v>
+      </c>
+      <c r="W14" t="s">
+        <v>32</v>
+      </c>
+      <c r="X14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0.51850890000000005</v>
+      </c>
+      <c r="AA14">
+        <v>0.96298229999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1655,46 +1892,67 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.53336810000000001</v>
+        <v>0.54144939999999997</v>
       </c>
       <c r="E15">
-        <v>0.89504989999999995</v>
+        <v>0.87640240000000003</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
       </c>
-      <c r="H15" t="s">
-        <v>9</v>
+      <c r="H15">
+        <v>0.47888429999999998</v>
       </c>
       <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>0.47914489999999998</v>
-      </c>
-      <c r="K15">
-        <v>1.0005553</v>
-      </c>
-      <c r="M15" t="s">
+        <v>0.99592639999999999</v>
+      </c>
+      <c r="K15" t="s">
         <v>20</v>
       </c>
-      <c r="N15" t="s">
-        <v>9</v>
-      </c>
-      <c r="O15">
-        <v>2</v>
+      <c r="L15">
+        <v>0.57716369999999995</v>
+      </c>
+      <c r="M15">
+        <v>0.80917570000000005</v>
+      </c>
+      <c r="O15" t="s">
+        <v>30</v>
       </c>
       <c r="P15">
-        <v>0.61157459999999997</v>
+        <v>0.68248180000000003</v>
       </c>
       <c r="Q15">
-        <v>0.73581549999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.6350365</v>
+      </c>
+      <c r="S15" t="s">
+        <v>31</v>
+      </c>
+      <c r="T15">
+        <v>0.49270069999999999</v>
+      </c>
+      <c r="U15">
+        <v>1.0145985</v>
+      </c>
+      <c r="W15" t="s">
+        <v>32</v>
+      </c>
+      <c r="X15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>0.53675700000000004</v>
+      </c>
+      <c r="AA15">
+        <v>0.92648589999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1702,46 +1960,67 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>0.52971849999999998</v>
+        <v>0.53336810000000001</v>
       </c>
       <c r="E16">
-        <v>0.9022635</v>
+        <v>0.89504989999999995</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
-      <c r="H16" t="s">
-        <v>9</v>
+      <c r="H16">
+        <v>0.47914489999999998</v>
       </c>
       <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <v>0.47888429999999998</v>
-      </c>
-      <c r="K16">
-        <v>1.0024666</v>
-      </c>
-      <c r="M16" t="s">
+        <v>1.0005553</v>
+      </c>
+      <c r="K16" t="s">
         <v>20</v>
       </c>
-      <c r="N16" t="s">
-        <v>9</v>
-      </c>
-      <c r="O16">
-        <v>3</v>
+      <c r="L16">
+        <v>0.57846719999999996</v>
+      </c>
+      <c r="M16">
+        <v>0.81031439999999999</v>
+      </c>
+      <c r="O16" t="s">
+        <v>30</v>
       </c>
       <c r="P16">
-        <v>0.61392080000000004</v>
+        <v>0.71611049999999998</v>
       </c>
       <c r="Q16">
-        <v>0.73378880000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.56777889999999998</v>
+      </c>
+      <c r="S16" t="s">
+        <v>31</v>
+      </c>
+      <c r="T16">
+        <v>0.46611049999999998</v>
+      </c>
+      <c r="U16">
+        <v>1.0677789</v>
+      </c>
+      <c r="W16" t="s">
+        <v>32</v>
+      </c>
+      <c r="X16" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y16">
+        <v>2</v>
+      </c>
+      <c r="Z16">
+        <v>0.54483839999999994</v>
+      </c>
+      <c r="AA16">
+        <v>0.91032329999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1749,46 +2028,67 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>0.52424400000000004</v>
+        <v>0.52971849999999998</v>
       </c>
       <c r="E17">
-        <v>0.91244150000000002</v>
+        <v>0.9022635</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
-      <c r="H17" t="s">
-        <v>9</v>
+      <c r="H17">
+        <v>0.47888429999999998</v>
       </c>
       <c r="I17">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>0.4804484</v>
-      </c>
-      <c r="K17">
-        <v>0.99928490000000003</v>
-      </c>
-      <c r="M17" t="s">
+        <v>1.0024666</v>
+      </c>
+      <c r="K17" t="s">
         <v>20</v>
       </c>
-      <c r="N17" t="s">
-        <v>9</v>
-      </c>
-      <c r="O17">
-        <v>4</v>
+      <c r="L17">
+        <v>0.58055270000000003</v>
+      </c>
+      <c r="M17">
+        <v>0.80716429999999995</v>
+      </c>
+      <c r="O17" t="s">
+        <v>30</v>
       </c>
       <c r="P17">
-        <v>0.61366010000000004</v>
+        <v>0.73826899999999995</v>
       </c>
       <c r="Q17">
-        <v>0.73544189999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.52346190000000004</v>
+      </c>
+      <c r="S17" t="s">
+        <v>31</v>
+      </c>
+      <c r="T17">
+        <v>0.45072990000000002</v>
+      </c>
+      <c r="U17">
+        <v>1.0985400999999999</v>
+      </c>
+      <c r="W17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y17">
+        <v>3</v>
+      </c>
+      <c r="Z17">
+        <v>0.54118869999999997</v>
+      </c>
+      <c r="AA17">
+        <v>0.91762250000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1796,46 +2096,67 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>0.52007300000000001</v>
+        <v>0.52424400000000004</v>
       </c>
       <c r="E18">
-        <v>0.9208421</v>
+        <v>0.91244150000000002</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
       </c>
-      <c r="H18" t="s">
-        <v>9</v>
+      <c r="H18">
+        <v>0.4804484</v>
       </c>
       <c r="I18">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <v>0.48175180000000001</v>
-      </c>
-      <c r="K18">
-        <v>0.99707009999999996</v>
-      </c>
-      <c r="M18" t="s">
+        <v>0.99928490000000003</v>
+      </c>
+      <c r="K18" t="s">
         <v>20</v>
       </c>
-      <c r="N18" t="s">
-        <v>9</v>
-      </c>
-      <c r="O18">
-        <v>5</v>
+      <c r="L18">
+        <v>0.58055270000000003</v>
+      </c>
+      <c r="M18">
+        <v>0.80663149999999995</v>
+      </c>
+      <c r="O18" t="s">
+        <v>30</v>
       </c>
       <c r="P18">
-        <v>0.61366010000000004</v>
+        <v>0.74504689999999996</v>
       </c>
       <c r="Q18">
-        <v>0.73492060000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.50990619999999998</v>
+      </c>
+      <c r="S18" t="s">
+        <v>31</v>
+      </c>
+      <c r="T18">
+        <v>0.45099060000000002</v>
+      </c>
+      <c r="U18">
+        <v>1.0980188</v>
+      </c>
+      <c r="W18" t="s">
+        <v>32</v>
+      </c>
+      <c r="X18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y18">
+        <v>4</v>
+      </c>
+      <c r="Z18">
+        <v>0.54588110000000001</v>
+      </c>
+      <c r="AA18">
+        <v>0.90823770000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1843,46 +2164,67 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>0.51642339999999998</v>
+        <v>0.52007300000000001</v>
       </c>
       <c r="E19">
-        <v>0.92812749999999999</v>
+        <v>0.9208421</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
       </c>
-      <c r="H19" t="s">
-        <v>9</v>
+      <c r="H19">
+        <v>0.48175180000000001</v>
       </c>
       <c r="I19">
-        <v>6</v>
-      </c>
-      <c r="J19">
-        <v>0.48175180000000001</v>
-      </c>
-      <c r="K19">
-        <v>0.99724069999999998</v>
-      </c>
-      <c r="M19" t="s">
+        <v>0.99707009999999996</v>
+      </c>
+      <c r="K19" t="s">
         <v>20</v>
       </c>
-      <c r="N19" t="s">
-        <v>9</v>
-      </c>
-      <c r="O19">
-        <v>6</v>
+      <c r="L19">
+        <v>0.58185609999999999</v>
+      </c>
+      <c r="M19">
+        <v>0.80455149999999998</v>
+      </c>
+      <c r="O19" t="s">
+        <v>30</v>
       </c>
       <c r="P19">
-        <v>0.61392080000000004</v>
+        <v>0.75521380000000005</v>
       </c>
       <c r="Q19">
-        <v>0.73453970000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.48957250000000002</v>
+      </c>
+      <c r="S19" t="s">
+        <v>31</v>
+      </c>
+      <c r="T19">
+        <v>0.455683</v>
+      </c>
+      <c r="U19">
+        <v>1.0886340000000001</v>
+      </c>
+      <c r="W19" t="s">
+        <v>32</v>
+      </c>
+      <c r="X19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+      <c r="Z19">
+        <v>0.54744530000000002</v>
+      </c>
+      <c r="AA19">
+        <v>0.90510950000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1890,46 +2232,67 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20">
-        <v>0.51381650000000001</v>
+        <v>0.51642339999999998</v>
       </c>
       <c r="E20">
-        <v>0.93293079999999995</v>
+        <v>0.92812749999999999</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
       </c>
-      <c r="H20" t="s">
-        <v>9</v>
+      <c r="H20">
+        <v>0.48175180000000001</v>
       </c>
       <c r="I20">
-        <v>7</v>
-      </c>
-      <c r="J20">
-        <v>0.48175180000000001</v>
-      </c>
-      <c r="K20">
-        <v>0.99722299999999997</v>
-      </c>
-      <c r="M20" t="s">
+        <v>0.99724069999999998</v>
+      </c>
+      <c r="K20" t="s">
         <v>20</v>
       </c>
-      <c r="N20" t="s">
-        <v>9</v>
-      </c>
-      <c r="O20">
-        <v>7</v>
+      <c r="L20">
+        <v>0.58185609999999999</v>
+      </c>
+      <c r="M20">
+        <v>0.80468819999999996</v>
+      </c>
+      <c r="O20" t="s">
+        <v>30</v>
       </c>
       <c r="P20">
-        <v>0.61287800000000003</v>
+        <v>0.75573509999999999</v>
       </c>
       <c r="Q20">
-        <v>0.73653860000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.48852970000000001</v>
+      </c>
+      <c r="S20" t="s">
+        <v>31</v>
+      </c>
+      <c r="T20">
+        <v>0.4554223</v>
+      </c>
+      <c r="U20">
+        <v>1.0891554000000001</v>
+      </c>
+      <c r="W20" t="s">
+        <v>32</v>
+      </c>
+      <c r="X20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y20">
+        <v>6</v>
+      </c>
+      <c r="Z20">
+        <v>0.54718460000000002</v>
+      </c>
+      <c r="AA20">
+        <v>0.90563090000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1937,46 +2300,67 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>0.51381650000000001</v>
       </c>
       <c r="E21">
-        <v>0.93296789999999996</v>
+        <v>0.93293079999999995</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
       </c>
-      <c r="H21" t="s">
-        <v>9</v>
+      <c r="H21">
+        <v>0.48175180000000001</v>
       </c>
       <c r="I21">
-        <v>8</v>
-      </c>
-      <c r="J21">
-        <v>0.48175180000000001</v>
-      </c>
-      <c r="K21">
-        <v>0.99726009999999998</v>
-      </c>
-      <c r="M21" t="s">
+        <v>0.99722299999999997</v>
+      </c>
+      <c r="K21" t="s">
         <v>20</v>
       </c>
-      <c r="N21" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21">
-        <v>8</v>
+      <c r="L21">
+        <v>0.58342020000000006</v>
+      </c>
+      <c r="M21">
+        <v>0.80200079999999996</v>
+      </c>
+      <c r="O21" t="s">
+        <v>30</v>
       </c>
       <c r="P21">
-        <v>0.61287800000000003</v>
+        <v>0.75782059999999996</v>
       </c>
       <c r="Q21">
-        <v>0.73654649999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.48435869999999998</v>
+      </c>
+      <c r="S21" t="s">
+        <v>31</v>
+      </c>
+      <c r="T21">
+        <v>0.4551616</v>
+      </c>
+      <c r="U21">
+        <v>1.0896767000000001</v>
+      </c>
+      <c r="W21" t="s">
+        <v>32</v>
+      </c>
+      <c r="X21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y21">
+        <v>7</v>
+      </c>
+      <c r="Z21">
+        <v>0.54692390000000002</v>
+      </c>
+      <c r="AA21">
+        <v>0.90615219999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1984,46 +2368,67 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>0.51381650000000001</v>
       </c>
       <c r="E22">
-        <v>0.93296730000000005</v>
+        <v>0.93296789999999996</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
-      <c r="H22" t="s">
-        <v>9</v>
+      <c r="H22">
+        <v>0.48175180000000001</v>
       </c>
       <c r="I22">
-        <v>9</v>
-      </c>
-      <c r="J22">
-        <v>0.48175180000000001</v>
-      </c>
-      <c r="K22">
         <v>0.99726009999999998</v>
       </c>
-      <c r="M22" t="s">
+      <c r="K22" t="s">
         <v>20</v>
       </c>
-      <c r="N22" t="s">
-        <v>9</v>
-      </c>
-      <c r="O22">
-        <v>9</v>
+      <c r="L22">
+        <v>0.58342020000000006</v>
+      </c>
+      <c r="M22">
+        <v>0.80203789999999997</v>
+      </c>
+      <c r="O22" t="s">
+        <v>30</v>
       </c>
       <c r="P22">
-        <v>0.61287800000000003</v>
+        <v>0.75782059999999996</v>
       </c>
       <c r="Q22">
-        <v>0.7365448</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.48435869999999998</v>
+      </c>
+      <c r="S22" t="s">
+        <v>31</v>
+      </c>
+      <c r="T22">
+        <v>0.45672580000000002</v>
+      </c>
+      <c r="U22">
+        <v>1.0865484999999999</v>
+      </c>
+      <c r="W22" t="s">
+        <v>32</v>
+      </c>
+      <c r="X22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y22">
+        <v>8</v>
+      </c>
+      <c r="Z22">
+        <v>0.54692390000000002</v>
+      </c>
+      <c r="AA22">
+        <v>0.90615219999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -2031,7 +2436,7 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23">
         <v>0.51381650000000001</v>
@@ -2042,32 +2447,121 @@
       <c r="G23" t="s">
         <v>14</v>
       </c>
-      <c r="H23" t="s">
-        <v>9</v>
+      <c r="H23">
+        <v>0.48175180000000001</v>
       </c>
       <c r="I23">
+        <v>0.99726009999999998</v>
+      </c>
+      <c r="K23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23">
+        <v>0.58342020000000006</v>
+      </c>
+      <c r="M23">
+        <v>0.80203729999999995</v>
+      </c>
+      <c r="O23" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23">
+        <v>0.75808129999999996</v>
+      </c>
+      <c r="Q23">
+        <v>0.48383730000000003</v>
+      </c>
+      <c r="S23" t="s">
+        <v>31</v>
+      </c>
+      <c r="T23">
+        <v>0.45672580000000002</v>
+      </c>
+      <c r="U23">
+        <v>1.0865484999999999</v>
+      </c>
+      <c r="W23" t="s">
+        <v>32</v>
+      </c>
+      <c r="X23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y23">
+        <v>9</v>
+      </c>
+      <c r="Z23">
+        <v>0.54692390000000002</v>
+      </c>
+      <c r="AA23">
+        <v>0.90615219999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
         <v>10</v>
       </c>
-      <c r="J23">
+      <c r="D24">
+        <v>0.51381650000000001</v>
+      </c>
+      <c r="E24">
+        <v>0.93296730000000005</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24">
         <v>0.48175180000000001</v>
       </c>
-      <c r="K23">
+      <c r="I24">
         <v>0.99726009999999998</v>
       </c>
-      <c r="M23" t="s">
+      <c r="K24" t="s">
         <v>20</v>
       </c>
-      <c r="N23" t="s">
-        <v>9</v>
-      </c>
-      <c r="O23">
+      <c r="L24">
+        <v>0.58342020000000006</v>
+      </c>
+      <c r="M24">
+        <v>0.80203729999999995</v>
+      </c>
+      <c r="O24" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24">
+        <v>0.75808129999999996</v>
+      </c>
+      <c r="Q24">
+        <v>0.48383730000000003</v>
+      </c>
+      <c r="S24" t="s">
+        <v>31</v>
+      </c>
+      <c r="T24">
+        <v>0.45672580000000002</v>
+      </c>
+      <c r="U24">
+        <v>1.0865484999999999</v>
+      </c>
+      <c r="W24" t="s">
+        <v>32</v>
+      </c>
+      <c r="X24" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y24">
         <v>10</v>
       </c>
-      <c r="P23">
-        <v>0.61287800000000003</v>
-      </c>
-      <c r="Q23">
-        <v>0.7365448</v>
+      <c r="Z24">
+        <v>0.54692390000000002</v>
+      </c>
+      <c r="AA24">
+        <v>0.90615219999999996</v>
       </c>
     </row>
   </sheetData>
@@ -2079,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,303 +2584,303 @@
     <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="9">
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8">
         <v>0.88800840000000003</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.45122269999999998</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.14023430000000001</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>0.16506129999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5">
         <v>0.86032070000000005</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.60135640000000001</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>0.16429659999999999</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>0.2168224</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
         <v>0.89027259999999997</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.65269619999999995</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.1763673</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>0.21945480000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
         <v>0.86445939999999999</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.82481749999999998</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.1839163</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>0.27108120000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="7" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5">
         <v>0.93695030000000001</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.65269619999999995</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.1763673</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>0.1260995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5">
         <v>0.89291259999999995</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.82481749999999998</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.1839163</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>0.2141749</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="10" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9">
         <v>0.94208829999999999</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.65269619999999995</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>0.1763673</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>0.11582340000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="9">
         <v>0.8942059</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0.82481749999999998</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.1839163</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>0.2115882</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="13" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="6">
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5">
         <v>0.96586260000000002</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>0.65269619999999995</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>0.1763673</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>6.8274799999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:6" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="6">
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5">
         <v>0.93998970000000004</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>0.82481749999999998</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>0.1839163</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>0.12002069999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="10">
+      <c r="B17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9">
         <v>0.94208829999999999</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>0.65269619999999995</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>4.4024300000000002E-2</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>0.11582340000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="9">
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="8">
         <v>0.8942059</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>0.82481749999999998</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>7.2845300000000002E-2</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>0.2115882</v>
       </c>
     </row>

</xml_diff>